<commit_message>
added auto scale axes
</commit_message>
<xml_diff>
--- a/acquisition_module/data/saved/saving.xlsx
+++ b/acquisition_module/data/saved/saving.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,22 +454,38 @@
           <t>value_TC_102</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>time_TC_103</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>value_TC_103</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.786799430847168</v>
+        <v>0.6210722923278809</v>
       </c>
       <c r="C2" t="n">
-        <v>23.7984594</v>
+        <v>8.19383378663189</v>
       </c>
       <c r="D2" t="n">
-        <v>0.786799430847168</v>
+        <v>0.6210722923278809</v>
       </c>
       <c r="E2" t="n">
-        <v>24.0713066</v>
+        <v>6.924113889145627</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.6210722923278809</v>
+      </c>
+      <c r="G2" t="n">
+        <v>28.22333742258084</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +493,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.642385482788086</v>
+        <v>1.118103265762329</v>
       </c>
       <c r="C3" t="n">
-        <v>23.7964031</v>
+        <v>16.09238665593796</v>
       </c>
       <c r="D3" t="n">
-        <v>1.642385482788086</v>
+        <v>1.118103265762329</v>
       </c>
       <c r="E3" t="n">
-        <v>24.0780293</v>
+        <v>31.4840098647054</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.118103265762329</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12.27960403431487</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +516,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2.325127601623535</v>
+        <v>1.618304252624512</v>
       </c>
       <c r="C4" t="n">
-        <v>23.7509878</v>
+        <v>7.780365476103739</v>
       </c>
       <c r="D4" t="n">
-        <v>2.325127601623535</v>
+        <v>1.618304252624512</v>
       </c>
       <c r="E4" t="n">
-        <v>24.0628057</v>
+        <v>21.69464588706281</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.618304252624512</v>
+      </c>
+      <c r="G4" t="n">
+        <v>14.77747326034588</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +539,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3.053734302520752</v>
+        <v>2.118157386779785</v>
       </c>
       <c r="C5" t="n">
-        <v>23.7865181</v>
+        <v>3.958621578138379</v>
       </c>
       <c r="D5" t="n">
-        <v>3.053734302520752</v>
+        <v>2.118157386779785</v>
       </c>
       <c r="E5" t="n">
-        <v>24.0672092</v>
+        <v>24.82862308104663</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.118157386779785</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20.75444070744295</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +562,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3.700688362121582</v>
+        <v>2.630987644195557</v>
       </c>
       <c r="C6" t="n">
-        <v>23.7698206</v>
+        <v>12.43128070429628</v>
       </c>
       <c r="D6" t="n">
-        <v>3.700688362121582</v>
+        <v>2.630987644195557</v>
       </c>
       <c r="E6" t="n">
-        <v>24.1967085</v>
+        <v>8.111408152830002</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.630987644195557</v>
+      </c>
+      <c r="G6" t="n">
+        <v>25.06965711356325</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +585,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>4.443059206008911</v>
+        <v>3.132695198059082</v>
       </c>
       <c r="C7" t="n">
-        <v>23.6930237</v>
+        <v>7.026233164209841</v>
       </c>
       <c r="D7" t="n">
-        <v>4.443059206008911</v>
+        <v>3.132695198059082</v>
       </c>
       <c r="E7" t="n">
-        <v>28.2069409</v>
+        <v>6.010812596750355</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.132695198059082</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8.860244642102899</v>
       </c>
     </row>
     <row r="8">
@@ -562,16 +608,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>5.150923728942871</v>
+        <v>3.635994434356689</v>
       </c>
       <c r="C8" t="n">
-        <v>23.6795277</v>
+        <v>12.83493925632031</v>
       </c>
       <c r="D8" t="n">
-        <v>5.150923728942871</v>
+        <v>3.635994434356689</v>
       </c>
       <c r="E8" t="n">
-        <v>29.1689159</v>
+        <v>24.85110075402243</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.635994434356689</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9.238392823812337</v>
       </c>
     </row>
     <row r="9">
@@ -579,16 +631,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>5.816107511520386</v>
+        <v>4.131721258163452</v>
       </c>
       <c r="C9" t="n">
-        <v>23.7345704</v>
+        <v>12.58618579491949</v>
       </c>
       <c r="D9" t="n">
-        <v>5.816107511520386</v>
+        <v>4.131721258163452</v>
       </c>
       <c r="E9" t="n">
-        <v>29.34104</v>
+        <v>39.85804674630723</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.131721258163452</v>
+      </c>
+      <c r="G9" t="n">
+        <v>18.49985577375569</v>
       </c>
     </row>
     <row r="10">
@@ -596,16 +654,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>6.508934020996094</v>
+        <v>4.634917497634888</v>
       </c>
       <c r="C10" t="n">
-        <v>23.7876086</v>
+        <v>11.21590177169928</v>
       </c>
       <c r="D10" t="n">
-        <v>6.508934020996094</v>
+        <v>4.634917497634888</v>
       </c>
       <c r="E10" t="n">
-        <v>29.503145</v>
+        <v>38.09328613412211</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.634917497634888</v>
+      </c>
+      <c r="G10" t="n">
+        <v>25.4193207227462</v>
       </c>
     </row>
     <row r="11">
@@ -613,220 +677,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>7.2077476978302</v>
+        <v>5.134474515914917</v>
       </c>
       <c r="C11" t="n">
-        <v>23.8047633</v>
+        <v>3.732059055599646</v>
       </c>
       <c r="D11" t="n">
-        <v>7.2077476978302</v>
+        <v>5.134474515914917</v>
       </c>
       <c r="E11" t="n">
-        <v>29.6391383</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>7.901597738265991</v>
-      </c>
-      <c r="C12" t="n">
-        <v>24.1974341</v>
-      </c>
-      <c r="D12" t="n">
-        <v>7.901597738265991</v>
-      </c>
-      <c r="E12" t="n">
-        <v>29.1867883</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>8.664886713027954</v>
-      </c>
-      <c r="C13" t="n">
-        <v>24.8421176</v>
-      </c>
-      <c r="D13" t="n">
-        <v>8.664886713027954</v>
-      </c>
-      <c r="E13" t="n">
-        <v>28.7046782</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>9.374643087387085</v>
-      </c>
-      <c r="C14" t="n">
-        <v>25.0882953</v>
-      </c>
-      <c r="D14" t="n">
-        <v>9.374643087387085</v>
-      </c>
-      <c r="E14" t="n">
-        <v>28.0313081</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>10.06963419914246</v>
-      </c>
-      <c r="C15" t="n">
-        <v>25.2987511</v>
-      </c>
-      <c r="D15" t="n">
-        <v>10.06963419914246</v>
-      </c>
-      <c r="E15" t="n">
-        <v>27.5513656</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>10.76787853240967</v>
-      </c>
-      <c r="C16" t="n">
-        <v>25.5191091</v>
-      </c>
-      <c r="D16" t="n">
-        <v>10.76787853240967</v>
-      </c>
-      <c r="E16" t="n">
-        <v>27.1431751</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>11.4649395942688</v>
-      </c>
-      <c r="C17" t="n">
-        <v>25.8298836</v>
-      </c>
-      <c r="D17" t="n">
-        <v>11.4649395942688</v>
-      </c>
-      <c r="E17" t="n">
-        <v>26.7582974</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>12.22345209121704</v>
-      </c>
-      <c r="C18" t="n">
-        <v>26.2551071</v>
-      </c>
-      <c r="D18" t="n">
-        <v>12.22345209121704</v>
-      </c>
-      <c r="E18" t="n">
-        <v>26.4692703</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>12.91671633720398</v>
-      </c>
-      <c r="C19" t="n">
-        <v>26.4571588</v>
-      </c>
-      <c r="D19" t="n">
-        <v>12.91671633720398</v>
-      </c>
-      <c r="E19" t="n">
-        <v>26.2629406</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>13.68061447143555</v>
-      </c>
-      <c r="C20" t="n">
-        <v>26.3229389</v>
-      </c>
-      <c r="D20" t="n">
-        <v>13.68061447143555</v>
-      </c>
-      <c r="E20" t="n">
-        <v>25.9607297</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>14.40618443489075</v>
-      </c>
-      <c r="C21" t="n">
-        <v>26.2511971</v>
-      </c>
-      <c r="D21" t="n">
-        <v>14.40618443489075</v>
-      </c>
-      <c r="E21" t="n">
-        <v>25.8031171</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>15.11884665489197</v>
-      </c>
-      <c r="C22" t="n">
-        <v>26.1126152</v>
-      </c>
-      <c r="D22" t="n">
-        <v>15.11884665489197</v>
-      </c>
-      <c r="E22" t="n">
-        <v>25.633016</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>15.84619832038879</v>
-      </c>
-      <c r="C23" t="n">
-        <v>25.989923</v>
-      </c>
-      <c r="D23" t="n">
-        <v>15.84619832038879</v>
-      </c>
-      <c r="E23" t="n">
-        <v>25.5190417</v>
+        <v>25.734025590337</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5.134474515914917</v>
+      </c>
+      <c r="G11" t="n">
+        <v>22.55258963974559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>